<commit_message>
Try catch block added
</commit_message>
<xml_diff>
--- a/Data/AgingMaturedTable.xlsx
+++ b/Data/AgingMaturedTable.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="112">
   <si>
     <t>Cust ID</t>
   </si>
@@ -43,226 +43,313 @@
     <t>Credit Amount</t>
   </si>
   <si>
-    <t>18030101254</t>
-  </si>
-  <si>
-    <t>90000000823</t>
-  </si>
-  <si>
-    <t>18030101576</t>
-  </si>
-  <si>
-    <t>90000043275</t>
-  </si>
-  <si>
-    <t>90000030746</t>
-  </si>
-  <si>
-    <t>18010119191</t>
-  </si>
-  <si>
-    <t>1803001366</t>
-  </si>
-  <si>
-    <t>18030104425</t>
-  </si>
-  <si>
-    <t>18010112922</t>
-  </si>
-  <si>
-    <t>18030099740</t>
-  </si>
-  <si>
-    <t>18030103129</t>
-  </si>
-  <si>
-    <t>90000042577</t>
-  </si>
-  <si>
-    <t>18030100574</t>
-  </si>
-  <si>
-    <t>18010119160</t>
-  </si>
-  <si>
-    <t>Shanti Pharmacy</t>
-  </si>
-  <si>
-    <t>Maa O Shisho General Hospital</t>
-  </si>
-  <si>
-    <t>Jom Jom Pharmacy</t>
-  </si>
-  <si>
-    <t>Jarina Salam Hospital</t>
-  </si>
-  <si>
-    <t>Peoples Private Hospital</t>
-  </si>
-  <si>
-    <t>Alfaz Medical Hall</t>
-  </si>
-  <si>
-    <t>Tamim Medical Hall</t>
-  </si>
-  <si>
-    <t>Suboj Pharmacy</t>
-  </si>
-  <si>
-    <t>Ahmed Oushad Ghar</t>
-  </si>
-  <si>
-    <t>S S Medical Hall</t>
-  </si>
-  <si>
-    <t>Dhaka Clinic</t>
-  </si>
-  <si>
-    <t>Akota General Private Hospital</t>
-  </si>
-  <si>
-    <t>Anika Medicine Corner</t>
-  </si>
-  <si>
-    <t>Al Modina Pharmacy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kalie Sree Para B Baria                                     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kamalpur Bhairab                                            </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jail Road B Baria                                           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shibpur Bazar Nabinagar B.Baria                             </t>
-  </si>
-  <si>
-    <t xml:space="preserve">C&amp;B Road Narsingdi                                          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fertilizer Gate Polash Narshingdi                           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Valanagar Narsingdi                                         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nilkoti Pagla Bazar                                         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">C &amp; B Road Narshingdi                                       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Potia NSD                                                   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Charsindur Bazar Ghorashal Polash Narsingdi                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Basail Narsingdi                                            </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Satirpara Narsingdi                                         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Station Road Narshingdi                                     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BB71                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BB33                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BB75                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BB22                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BB62                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BB12                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BB21                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BB11                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV180-382188     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV180-377834     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV180-373204     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV180-392594     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV180-393080     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV180-381472     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV180-381648     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV180-382159     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV180-382336     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV180-382243     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV180-382894     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV180-394698     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV180-382451     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV180-388541     </t>
-  </si>
-  <si>
-    <t>02 Sep 2020</t>
-  </si>
-  <si>
-    <t>20 Aug 2020</t>
-  </si>
-  <si>
-    <t>08 Aug 2020</t>
+    <t>90000028229</t>
+  </si>
+  <si>
+    <t>90000025494</t>
+  </si>
+  <si>
+    <t>44037801632</t>
+  </si>
+  <si>
+    <t>44019001487</t>
+  </si>
+  <si>
+    <t>44019000528</t>
+  </si>
+  <si>
+    <t>90000025671</t>
+  </si>
+  <si>
+    <t>90000041678</t>
+  </si>
+  <si>
+    <t>44031000794</t>
+  </si>
+  <si>
+    <t>44019004795</t>
+  </si>
+  <si>
+    <t>44019001544</t>
+  </si>
+  <si>
+    <t>44019003218</t>
+  </si>
+  <si>
+    <t>90000029246</t>
+  </si>
+  <si>
+    <t>4401900199</t>
+  </si>
+  <si>
+    <t>44031102640</t>
+  </si>
+  <si>
+    <t>90000033723</t>
+  </si>
+  <si>
+    <t>90000043217</t>
+  </si>
+  <si>
+    <t>4401900145</t>
+  </si>
+  <si>
+    <t>4401900743</t>
+  </si>
+  <si>
+    <t>90000015767</t>
+  </si>
+  <si>
+    <t>90000035764</t>
+  </si>
+  <si>
+    <t>Bondhon Hospital</t>
+  </si>
+  <si>
+    <t>Maa Medicine Corner</t>
+  </si>
+  <si>
+    <t>Tahsin Pharmacy</t>
+  </si>
+  <si>
+    <t>Shikder Pharmacy</t>
+  </si>
+  <si>
+    <t>Dr. Arobindu</t>
+  </si>
+  <si>
+    <t>SKH Pharmacy</t>
+  </si>
+  <si>
+    <t>Sarder Medicine Corner</t>
+  </si>
+  <si>
+    <t>Dr Akber Hossain</t>
+  </si>
+  <si>
+    <t>Mubin Pharmacy</t>
+  </si>
+  <si>
+    <t>Lily Pharmacy</t>
+  </si>
+  <si>
+    <t>Aritra Pharmacy</t>
+  </si>
+  <si>
+    <t>Al Nur Hospital</t>
+  </si>
+  <si>
+    <t>Tanny Pharmacy</t>
+  </si>
+  <si>
+    <t>Shahana Clinic</t>
+  </si>
+  <si>
+    <t>Musaffa Medicine Shop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Janoni Pharmacy </t>
+  </si>
+  <si>
+    <t>Rudra Pharmacy</t>
+  </si>
+  <si>
+    <t>Zaman Pharmacy</t>
+  </si>
+  <si>
+    <t>Morol Pharmacy</t>
+  </si>
+  <si>
+    <t>Foraze Medical Hall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">96,Jail Road, Jessore                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paira Bazar, Noapara                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nowabeki Bazar Shyamnagar Satkhira                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Narkelbaria Bagharpara Jessore                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bagaharpara Jessore                                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Makrail Bazar,Lohagora                                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hospital road,Noapara,Jessore                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boro Gabura Bazar Shyamnagar Satkhira                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monirampur Bazar Jessore                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monirampur Jessore                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Khajura Bazar Jessore                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Khulna road,Satkhira                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Narkel Baria Jessore                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Noornagar Bazar Noornagar Shamnagar Satkhira                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Koikhali,Zada Bazar,Shyamnagor                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pulerhat bazar, Khajura, Bagherpara                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Narikalbaria Bahgarpara Jessore                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hasanpur Bazar Keshobpur                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sakhiripota Bazar,Navaron                                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benapole Port,Sharsha                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JS22                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JS71                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JS82                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JS24                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JS32                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JS75                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JS81                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JS73                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JS51                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JS84                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JS72                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JS64                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV440-328103     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV440-463904     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV440-464492     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV440-465521     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV440-465464     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV440-465727     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV440-465744     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV440-465010     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV440-466471     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV440-467048     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV440-467308     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV440-445659     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV440-468655     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV440-469543     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV440-470604     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV440-470491     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV440-470160     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV440-470372     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV440-470850     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV440-470846     </t>
+  </si>
+  <si>
+    <t>04 Nov 2019</t>
+  </si>
+  <si>
+    <t>15 Sep 2020</t>
+  </si>
+  <si>
+    <t>16 Sep 2020</t>
+  </si>
+  <si>
+    <t>18 Sep 2020</t>
+  </si>
+  <si>
+    <t>19 Sep 2020</t>
+  </si>
+  <si>
+    <t>21 Sep 2020</t>
+  </si>
+  <si>
+    <t>10 Aug 2020</t>
+  </si>
+  <si>
+    <t>25 Sep 2020</t>
+  </si>
+  <si>
+    <t>26 Sep 2020</t>
+  </si>
+  <si>
+    <t>28 Sep 2020</t>
   </si>
   <si>
     <t>29 Sep 2020</t>
-  </si>
-  <si>
-    <t>30 Sep 2020</t>
-  </si>
-  <si>
-    <t>31 Aug 2020</t>
-  </si>
-  <si>
-    <t>01 Sep 2020</t>
-  </si>
-  <si>
-    <t>03 Sep 2020</t>
-  </si>
-  <si>
-    <t>04 Oct 2020</t>
-  </si>
-  <si>
-    <t>18 Sep 2020</t>
   </si>
 </sst>
 </file>
@@ -620,7 +707,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -663,28 +750,28 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="E2" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="F2" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="G2" t="s">
-        <v>73</v>
+        <v>101</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="I2">
-        <v>47</v>
+        <v>305</v>
       </c>
       <c r="J2">
-        <v>19824.04</v>
+        <v>37965.05</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -695,28 +782,28 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="E3" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="F3" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="G3" t="s">
-        <v>74</v>
+        <v>102</v>
       </c>
       <c r="H3">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I3">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="J3">
-        <v>14783.35</v>
+        <v>7225.06</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -727,28 +814,28 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="E4" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="F4" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="G4" t="s">
-        <v>75</v>
+        <v>103</v>
       </c>
       <c r="H4">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="J4">
-        <v>14946.69</v>
+        <v>29785.03</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -759,28 +846,28 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="E5" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="F5" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="G5" t="s">
-        <v>76</v>
+        <v>104</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="J5">
-        <v>34656.47</v>
+        <v>10015.45</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -791,28 +878,28 @@
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="E6" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="F6" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="G6" t="s">
-        <v>77</v>
+        <v>104</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="J6">
-        <v>50217.16</v>
+        <v>5018.94</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -823,28 +910,28 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E7" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="F7" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="G7" t="s">
-        <v>78</v>
+        <v>105</v>
       </c>
       <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
         <v>30</v>
       </c>
-      <c r="I7">
-        <v>19</v>
-      </c>
       <c r="J7">
-        <v>4462.45</v>
+        <v>9232.5</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -855,28 +942,28 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="E8" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="F8" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="G8" t="s">
-        <v>78</v>
+        <v>105</v>
       </c>
       <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
         <v>30</v>
       </c>
-      <c r="I8">
-        <v>19</v>
-      </c>
       <c r="J8">
-        <v>4360.16</v>
+        <v>9000</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -887,28 +974,28 @@
         <v>16</v>
       </c>
       <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" t="s">
+        <v>88</v>
+      </c>
+      <c r="G9" t="s">
+        <v>105</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
         <v>30</v>
       </c>
-      <c r="D9" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" t="s">
-        <v>52</v>
-      </c>
-      <c r="F9" t="s">
-        <v>66</v>
-      </c>
-      <c r="G9" t="s">
-        <v>79</v>
-      </c>
-      <c r="H9">
-        <v>30</v>
-      </c>
-      <c r="I9">
-        <v>18</v>
-      </c>
       <c r="J9">
-        <v>4929.08</v>
+        <v>4600</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -919,28 +1006,28 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="E10" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="F10" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="G10" t="s">
-        <v>73</v>
+        <v>106</v>
       </c>
       <c r="H10">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I10">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="J10">
-        <v>9977.469999999999</v>
+        <v>14756.66</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -951,28 +1038,28 @@
         <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="E11" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="F11" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="G11" t="s">
-        <v>73</v>
+        <v>106</v>
       </c>
       <c r="H11">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I11">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="J11">
-        <v>6937.07</v>
+        <v>12174.16</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -983,28 +1070,28 @@
         <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D12" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="E12" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="F12" t="s">
-        <v>69</v>
+        <v>91</v>
       </c>
       <c r="G12" t="s">
-        <v>80</v>
+        <v>106</v>
       </c>
       <c r="H12">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I12">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="J12">
-        <v>5092.56</v>
+        <v>8507.01</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -1015,28 +1102,28 @@
         <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="D13" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="E13" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F13" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="G13" t="s">
-        <v>81</v>
+        <v>107</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="I13">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="J13">
-        <v>22108.11</v>
+        <v>19193.25</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1047,28 +1134,28 @@
         <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="D14" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="E14" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="F14" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="G14" t="s">
-        <v>73</v>
+        <v>108</v>
       </c>
       <c r="H14">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="I14">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="J14">
-        <v>10495.53</v>
+        <v>5981.62</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1079,28 +1166,220 @@
         <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="D15" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="E15" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="F15" t="s">
+        <v>94</v>
+      </c>
+      <c r="G15" t="s">
+        <v>109</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>23</v>
+      </c>
+      <c r="J15">
+        <v>15081.07</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" t="s">
+        <v>75</v>
+      </c>
+      <c r="F16" t="s">
+        <v>95</v>
+      </c>
+      <c r="G16" t="s">
+        <v>110</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>21</v>
+      </c>
+      <c r="J16">
+        <v>15146.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" t="s">
         <v>72</v>
       </c>
-      <c r="G15" t="s">
-        <v>82</v>
-      </c>
-      <c r="H15">
-        <v>30</v>
-      </c>
-      <c r="I15">
-        <v>1</v>
-      </c>
-      <c r="J15">
-        <v>9952.700000000001</v>
+      <c r="F17" t="s">
+        <v>96</v>
+      </c>
+      <c r="G17" t="s">
+        <v>110</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>21</v>
+      </c>
+      <c r="J17">
+        <v>15062.62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18" t="s">
+        <v>72</v>
+      </c>
+      <c r="F18" t="s">
+        <v>97</v>
+      </c>
+      <c r="G18" t="s">
+        <v>110</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>21</v>
+      </c>
+      <c r="J18">
+        <v>6069.21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" t="s">
+        <v>79</v>
+      </c>
+      <c r="F19" t="s">
+        <v>98</v>
+      </c>
+      <c r="G19" t="s">
+        <v>110</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>21</v>
+      </c>
+      <c r="J19">
+        <v>4693.52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" t="s">
+        <v>80</v>
+      </c>
+      <c r="F20" t="s">
+        <v>99</v>
+      </c>
+      <c r="G20" t="s">
+        <v>111</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>20</v>
+      </c>
+      <c r="J20">
+        <v>10450.76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" t="s">
+        <v>80</v>
+      </c>
+      <c r="F21" t="s">
+        <v>100</v>
+      </c>
+      <c r="G21" t="s">
+        <v>111</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>20</v>
+      </c>
+      <c r="J21">
+        <v>10073.41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Full dynamic functionality tested
</commit_message>
<xml_diff>
--- a/Data/AgingMaturedTable.xlsx
+++ b/Data/AgingMaturedTable.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="108">
   <si>
     <t>Cust ID</t>
   </si>
@@ -43,313 +43,301 @@
     <t>Credit Amount</t>
   </si>
   <si>
-    <t>90000028229</t>
-  </si>
-  <si>
-    <t>90000025494</t>
-  </si>
-  <si>
-    <t>44037801632</t>
-  </si>
-  <si>
-    <t>44019001487</t>
-  </si>
-  <si>
-    <t>44019000528</t>
-  </si>
-  <si>
-    <t>90000025671</t>
-  </si>
-  <si>
-    <t>90000041678</t>
-  </si>
-  <si>
-    <t>44031000794</t>
-  </si>
-  <si>
-    <t>44019004795</t>
-  </si>
-  <si>
-    <t>44019001544</t>
-  </si>
-  <si>
-    <t>44019003218</t>
-  </si>
-  <si>
-    <t>90000029246</t>
-  </si>
-  <si>
-    <t>4401900199</t>
-  </si>
-  <si>
-    <t>44031102640</t>
-  </si>
-  <si>
-    <t>90000033723</t>
-  </si>
-  <si>
-    <t>90000043217</t>
-  </si>
-  <si>
-    <t>4401900145</t>
-  </si>
-  <si>
-    <t>4401900743</t>
-  </si>
-  <si>
-    <t>90000015767</t>
-  </si>
-  <si>
-    <t>90000035764</t>
-  </si>
-  <si>
-    <t>Bondhon Hospital</t>
-  </si>
-  <si>
-    <t>Maa Medicine Corner</t>
-  </si>
-  <si>
-    <t>Tahsin Pharmacy</t>
-  </si>
-  <si>
-    <t>Shikder Pharmacy</t>
-  </si>
-  <si>
-    <t>Dr. Arobindu</t>
-  </si>
-  <si>
-    <t>SKH Pharmacy</t>
-  </si>
-  <si>
-    <t>Sarder Medicine Corner</t>
-  </si>
-  <si>
-    <t>Dr Akber Hossain</t>
-  </si>
-  <si>
-    <t>Mubin Pharmacy</t>
-  </si>
-  <si>
-    <t>Lily Pharmacy</t>
-  </si>
-  <si>
-    <t>Aritra Pharmacy</t>
-  </si>
-  <si>
-    <t>Al Nur Hospital</t>
-  </si>
-  <si>
-    <t>Tanny Pharmacy</t>
-  </si>
-  <si>
-    <t>Shahana Clinic</t>
-  </si>
-  <si>
-    <t>Musaffa Medicine Shop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Janoni Pharmacy </t>
-  </si>
-  <si>
-    <t>Rudra Pharmacy</t>
-  </si>
-  <si>
-    <t>Zaman Pharmacy</t>
-  </si>
-  <si>
-    <t>Morol Pharmacy</t>
-  </si>
-  <si>
-    <t>Foraze Medical Hall</t>
-  </si>
-  <si>
-    <t xml:space="preserve">96,Jail Road, Jessore                                       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paira Bazar, Noapara                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nowabeki Bazar Shyamnagar Satkhira                          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Narkelbaria Bagharpara Jessore                              </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bagaharpara Jessore                                         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Makrail Bazar,Lohagora                                      </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hospital road,Noapara,Jessore                               </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Boro Gabura Bazar Shyamnagar Satkhira                       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monirampur Bazar Jessore                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monirampur Jessore                                          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Khajura Bazar Jessore                                       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Khulna road,Satkhira                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Narkel Baria Jessore                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Noornagar Bazar Noornagar Shamnagar Satkhira                </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Koikhali,Zada Bazar,Shyamnagor                              </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pulerhat bazar, Khajura, Bagherpara                         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Narikalbaria Bahgarpara Jessore                             </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hasanpur Bazar Keshobpur                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sakhiripota Bazar,Navaron                                   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Benapole Port,Sharsha                                       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">JS22                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">JS71                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">JS82                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">JS24                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">JS32                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">JS75                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">JS81                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">JS73                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">JS51                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">JS84                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">JS72                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">JS64                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV440-328103     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV440-463904     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV440-464492     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV440-465521     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV440-465464     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV440-465727     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV440-465744     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV440-465010     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV440-466471     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV440-467048     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV440-467308     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV440-445659     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV440-468655     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV440-469543     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV440-470604     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV440-470491     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV440-470160     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV440-470372     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV440-470850     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV440-470846     </t>
-  </si>
-  <si>
-    <t>04 Nov 2019</t>
-  </si>
-  <si>
-    <t>15 Sep 2020</t>
-  </si>
-  <si>
-    <t>16 Sep 2020</t>
+    <t>12010508678</t>
+  </si>
+  <si>
+    <t>12010506029</t>
+  </si>
+  <si>
+    <t>90000017057</t>
+  </si>
+  <si>
+    <t>12010508403</t>
+  </si>
+  <si>
+    <t>12010503383</t>
+  </si>
+  <si>
+    <t>90000008868</t>
+  </si>
+  <si>
+    <t>12010500942</t>
+  </si>
+  <si>
+    <t>12010126256</t>
+  </si>
+  <si>
+    <t>90000024109</t>
+  </si>
+  <si>
+    <t>12010111044</t>
+  </si>
+  <si>
+    <t>12010508887</t>
+  </si>
+  <si>
+    <t>90000037169</t>
+  </si>
+  <si>
+    <t>90000001383</t>
+  </si>
+  <si>
+    <t>12010121170</t>
+  </si>
+  <si>
+    <t>90000039670</t>
+  </si>
+  <si>
+    <t>12010505858</t>
+  </si>
+  <si>
+    <t>Emon Drag House</t>
+  </si>
+  <si>
+    <t>Dream Pharma</t>
+  </si>
+  <si>
+    <t>Dhaka Central Diagnostic &amp; Ima</t>
+  </si>
+  <si>
+    <t>Dhaka Central Int. Medical Col</t>
+  </si>
+  <si>
+    <t>Badas Pharmacy  NHN   DAB</t>
+  </si>
+  <si>
+    <t>Health Labs Pharmacy</t>
+  </si>
+  <si>
+    <t>Marie Stopes Clinic</t>
+  </si>
+  <si>
+    <t>Marks ENT Hospital  Institutio</t>
+  </si>
+  <si>
+    <t>Nurunnahar Pharmacy</t>
+  </si>
+  <si>
+    <t>R  K  Medical Hall</t>
+  </si>
+  <si>
+    <t>Shah Ali Pharmacy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mr.Rafiqul Islam  AIC </t>
+  </si>
+  <si>
+    <t>M  Hassan Pharmacy</t>
+  </si>
+  <si>
+    <t>Bangladesh Eye Hospital Mirpur</t>
+  </si>
+  <si>
+    <t>OSB Chasma Ghar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C 11 12 shah Ali girls College,Mirpur 1,Dhaka               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mirpur 10 A,Beside of Diginova,Dhaka                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">38/1, Ring Road,Shaymoli                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 1,Ring Road,Shymoly,Dhaka                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Main Road,Mirpur  10,Dhaka                                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">East,Shewrapara,Near Sohel Pharmacy                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mirpur 10,Opposite Indoor Stadium,Mirpur,Dhaka              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mirpur 14,Dhaka                                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">House-3, Road No-2,Block-E, Kalsi Road, Mirpur-11, Dhaka    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Satter Market,Dhaka Cantonment,Dhaka                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bouniabad,Mirpur   11                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shah Ali Bag Mirpur 1,Dhaka                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TDCL, Mirpur                                                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">83, Pal Para Golar Tak,Mirpur   1,Dhaka                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">66 Sumi Tower Zoo Road Mirpur 2 Dhaka                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mirpur  2,Dhaka                                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DM21                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DM61                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ND12                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DM44                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DM14                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">UM44                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DM63                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">UM43                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DM64                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DM31                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INST                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DM22                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DM43                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DM52                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV115-350114     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV115-527072     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV115-564683     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV115-565405     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV115-568933     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV115-589486     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV115-579025     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV115-669401     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV115-642893     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV115-611934     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV115-583159     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV115-644928     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV115-658462     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV115-658961     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV115-677980     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV115-678190     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV115-679076     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV115-663520     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV115-644970     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV115-646039     </t>
+  </si>
+  <si>
+    <t>18 Feb 2019</t>
+  </si>
+  <si>
+    <t>16 Jan 2020</t>
+  </si>
+  <si>
+    <t>21 Mar 2020</t>
+  </si>
+  <si>
+    <t>22 Mar 2020</t>
+  </si>
+  <si>
+    <t>28 Mar 2020</t>
+  </si>
+  <si>
+    <t>09 May 2020</t>
+  </si>
+  <si>
+    <t>18 Apr 2020</t>
   </si>
   <si>
     <t>18 Sep 2020</t>
   </si>
   <si>
-    <t>19 Sep 2020</t>
-  </si>
-  <si>
-    <t>21 Sep 2020</t>
+    <t>06 Aug 2020</t>
+  </si>
+  <si>
+    <t>16 Jun 2020</t>
+  </si>
+  <si>
+    <t>27 Apr 2020</t>
   </si>
   <si>
     <t>10 Aug 2020</t>
   </si>
   <si>
-    <t>25 Sep 2020</t>
-  </si>
-  <si>
-    <t>26 Sep 2020</t>
-  </si>
-  <si>
-    <t>28 Sep 2020</t>
-  </si>
-  <si>
-    <t>29 Sep 2020</t>
+    <t>31 Aug 2020</t>
+  </si>
+  <si>
+    <t>01 Sep 2020</t>
+  </si>
+  <si>
+    <t>02 Oct 2020</t>
+  </si>
+  <si>
+    <t>04 Oct 2020</t>
+  </si>
+  <si>
+    <t>08 Sep 2020</t>
+  </si>
+  <si>
+    <t>12 Aug 2020</t>
   </si>
 </sst>
 </file>
@@ -750,28 +738,28 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="E2" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="F2" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="G2" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="H2">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="I2">
-        <v>305</v>
+        <v>579</v>
       </c>
       <c r="J2">
-        <v>37965.05</v>
+        <v>20124.56</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -782,28 +770,28 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E3" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="F3" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="G3" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="I3">
-        <v>34</v>
+        <v>232</v>
       </c>
       <c r="J3">
-        <v>7225.06</v>
+        <v>30531</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -814,28 +802,28 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="E4" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="F4" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="G4" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="I4">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="J4">
-        <v>29785.03</v>
+        <v>1548.97</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -846,28 +834,28 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="E5" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="F5" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="G5" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="I5">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="J5">
-        <v>10015.45</v>
+        <v>7068</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -875,31 +863,31 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="E6" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="F6" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="G6" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="I6">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="J6">
-        <v>5018.94</v>
+        <v>3991.58</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -907,31 +895,31 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="E7" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="F7" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="G7" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="I7">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="J7">
-        <v>9232.5</v>
+        <v>11127.07</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -939,31 +927,31 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E8" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="F8" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="G8" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="I8">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="J8">
-        <v>9000</v>
+        <v>1854.52</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -971,31 +959,31 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="E9" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="F9" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="G9" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="I9">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J9">
-        <v>4600</v>
+        <v>10010</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1003,31 +991,31 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" t="s">
         <v>57</v>
       </c>
-      <c r="E10" t="s">
-        <v>76</v>
-      </c>
       <c r="F10" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="G10" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="I10">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J10">
-        <v>14756.66</v>
+        <v>854</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1035,31 +1023,31 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="E11" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="F11" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="G11" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I11">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J11">
-        <v>12174.16</v>
+        <v>83834.25999999999</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -1067,31 +1055,31 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="D12" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="E12" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="F12" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="G12" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="I12">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J12">
-        <v>8507.01</v>
+        <v>3431</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -1099,22 +1087,22 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D13" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="E13" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="F13" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="G13" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="H13">
         <v>45</v>
@@ -1123,7 +1111,7 @@
         <v>25</v>
       </c>
       <c r="J13">
-        <v>19193.25</v>
+        <v>90.97</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1131,31 +1119,31 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D14" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="E14" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F14" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="G14" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="I14">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="J14">
-        <v>5981.62</v>
+        <v>17000</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1163,31 +1151,31 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D15" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="E15" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="F15" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="G15" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="I15">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="J15">
-        <v>15081.07</v>
+        <v>17540.62</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1195,31 +1183,31 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D16" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="E16" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="F16" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="G16" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="H16">
         <v>0</v>
       </c>
       <c r="I16">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="J16">
-        <v>15146.4</v>
+        <v>9461.07</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1227,31 +1215,31 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D17" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="E17" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F17" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="G17" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="H17">
         <v>0</v>
       </c>
       <c r="I17">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="J17">
-        <v>15062.62</v>
+        <v>369.62</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1259,31 +1247,31 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D18" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="E18" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F18" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="G18" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="H18">
         <v>0</v>
       </c>
       <c r="I18">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="J18">
-        <v>6069.21</v>
+        <v>2136.05</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1291,31 +1279,31 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C19" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="D19" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="E19" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="F19" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="G19" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="H19">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="I19">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="J19">
-        <v>4693.52</v>
+        <v>7500</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1323,31 +1311,31 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D20" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="E20" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="F20" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="G20" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="I20">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="J20">
-        <v>10450.76</v>
+        <v>10804.62</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1355,31 +1343,31 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D21" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="E21" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="F21" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="G21" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="H21">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="I21">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J21">
-        <v>10073.41</v>
+        <v>17657.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add functionality for all reports in a particular NDM
</commit_message>
<xml_diff>
--- a/Data/AgingMaturedTable.xlsx
+++ b/Data/AgingMaturedTable.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="120">
   <si>
     <t>Cust ID</t>
   </si>
@@ -43,301 +43,337 @@
     <t>Credit Amount</t>
   </si>
   <si>
-    <t>12010508678</t>
-  </si>
-  <si>
-    <t>12010506029</t>
-  </si>
-  <si>
-    <t>90000017057</t>
-  </si>
-  <si>
-    <t>12010508403</t>
-  </si>
-  <si>
-    <t>12010503383</t>
-  </si>
-  <si>
-    <t>90000008868</t>
-  </si>
-  <si>
-    <t>12010500942</t>
-  </si>
-  <si>
-    <t>12010126256</t>
-  </si>
-  <si>
-    <t>90000024109</t>
-  </si>
-  <si>
-    <t>12010111044</t>
-  </si>
-  <si>
-    <t>12010508887</t>
-  </si>
-  <si>
-    <t>90000037169</t>
-  </si>
-  <si>
-    <t>90000001383</t>
-  </si>
-  <si>
-    <t>12010121170</t>
-  </si>
-  <si>
-    <t>90000039670</t>
-  </si>
-  <si>
-    <t>12010505858</t>
-  </si>
-  <si>
-    <t>Emon Drag House</t>
-  </si>
-  <si>
-    <t>Dream Pharma</t>
-  </si>
-  <si>
-    <t>Dhaka Central Diagnostic &amp; Ima</t>
-  </si>
-  <si>
-    <t>Dhaka Central Int. Medical Col</t>
-  </si>
-  <si>
-    <t>Badas Pharmacy  NHN   DAB</t>
-  </si>
-  <si>
-    <t>Health Labs Pharmacy</t>
-  </si>
-  <si>
-    <t>Marie Stopes Clinic</t>
-  </si>
-  <si>
-    <t>Marks ENT Hospital  Institutio</t>
-  </si>
-  <si>
-    <t>Nurunnahar Pharmacy</t>
-  </si>
-  <si>
-    <t>R  K  Medical Hall</t>
-  </si>
-  <si>
-    <t>Shah Ali Pharmacy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mr.Rafiqul Islam  AIC </t>
-  </si>
-  <si>
-    <t>M  Hassan Pharmacy</t>
-  </si>
-  <si>
-    <t>Bangladesh Eye Hospital Mirpur</t>
-  </si>
-  <si>
-    <t>OSB Chasma Ghar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C 11 12 shah Ali girls College,Mirpur 1,Dhaka               </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mirpur 10 A,Beside of Diginova,Dhaka                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">38/1, Ring Road,Shaymoli                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 1,Ring Road,Shymoly,Dhaka                                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Main Road,Mirpur  10,Dhaka                                  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">East,Shewrapara,Near Sohel Pharmacy                         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mirpur 10,Opposite Indoor Stadium,Mirpur,Dhaka              </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mirpur 14,Dhaka                                             </t>
-  </si>
-  <si>
-    <t xml:space="preserve">House-3, Road No-2,Block-E, Kalsi Road, Mirpur-11, Dhaka    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Satter Market,Dhaka Cantonment,Dhaka                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bouniabad,Mirpur   11                                       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shah Ali Bag Mirpur 1,Dhaka                                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TDCL, Mirpur                                                </t>
-  </si>
-  <si>
-    <t xml:space="preserve">83, Pal Para Golar Tak,Mirpur   1,Dhaka                     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">66 Sumi Tower Zoo Road Mirpur 2 Dhaka                       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mirpur  2,Dhaka                                             </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DM21                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DM61                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ND12                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DM44                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DM14                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">UM44                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DM63                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">UM43                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DM64                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DM31                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">INST                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DM22                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DM43                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DM52                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV115-350114     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV115-527072     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV115-564683     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV115-565405     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV115-568933     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV115-589486     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV115-579025     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV115-669401     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV115-642893     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV115-611934     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV115-583159     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV115-644928     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV115-658462     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV115-658961     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV115-677980     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV115-678190     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV115-679076     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV115-663520     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV115-644970     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV115-646039     </t>
-  </si>
-  <si>
-    <t>18 Feb 2019</t>
-  </si>
-  <si>
-    <t>16 Jan 2020</t>
-  </si>
-  <si>
-    <t>21 Mar 2020</t>
-  </si>
-  <si>
-    <t>22 Mar 2020</t>
-  </si>
-  <si>
-    <t>28 Mar 2020</t>
-  </si>
-  <si>
-    <t>09 May 2020</t>
-  </si>
-  <si>
-    <t>18 Apr 2020</t>
+    <t>90000028229</t>
+  </si>
+  <si>
+    <t>90000014597</t>
+  </si>
+  <si>
+    <t>44019001544</t>
+  </si>
+  <si>
+    <t>90000029246</t>
+  </si>
+  <si>
+    <t>44031106594</t>
+  </si>
+  <si>
+    <t>4406114678</t>
+  </si>
+  <si>
+    <t>44019008675</t>
+  </si>
+  <si>
+    <t>44037801992</t>
+  </si>
+  <si>
+    <t>44037801368</t>
+  </si>
+  <si>
+    <t>90000003945</t>
+  </si>
+  <si>
+    <t>44031000237</t>
+  </si>
+  <si>
+    <t>44019001016</t>
+  </si>
+  <si>
+    <t>44019003221</t>
+  </si>
+  <si>
+    <t>44019003034</t>
+  </si>
+  <si>
+    <t>44031106947</t>
+  </si>
+  <si>
+    <t>44031000626</t>
+  </si>
+  <si>
+    <t>44019003399</t>
+  </si>
+  <si>
+    <t>90000018632</t>
+  </si>
+  <si>
+    <t>44019002997</t>
+  </si>
+  <si>
+    <t>44019001746</t>
+  </si>
+  <si>
+    <t>Bondhon Hospital</t>
+  </si>
+  <si>
+    <t>Litu Pharmacy</t>
+  </si>
+  <si>
+    <t>Lily Pharmacy</t>
+  </si>
+  <si>
+    <t>Al Nur Hospital</t>
+  </si>
+  <si>
+    <t>Gazi Pharmacy</t>
+  </si>
+  <si>
+    <t>Popular Pharmacy</t>
+  </si>
+  <si>
+    <t>Ibn Sina Diagnostic Center</t>
+  </si>
+  <si>
+    <t>Sher E Bangla Clinic</t>
+  </si>
+  <si>
+    <t>Ram Krishna pharmacy</t>
+  </si>
+  <si>
+    <t>Dalia Clinic</t>
+  </si>
+  <si>
+    <t>National Medical Hall</t>
+  </si>
+  <si>
+    <t>Raju Pharmacy</t>
+  </si>
+  <si>
+    <t>Shorif Pharmacy</t>
+  </si>
+  <si>
+    <t>Das Pharmacy</t>
+  </si>
+  <si>
+    <t>Rojina Pharmacy</t>
+  </si>
+  <si>
+    <t>Janoni Pharmacy</t>
+  </si>
+  <si>
+    <t>Bikalpo Pharmacy</t>
+  </si>
+  <si>
+    <t>China Bangla  CB  Hospital</t>
+  </si>
+  <si>
+    <t>Al Muaz Pharmacy</t>
+  </si>
+  <si>
+    <t>Matree Medical Hall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">96,Jail Road, Jessore                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manderbaria Bazar,Kaligonj,Jhenaidah                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monirampur Jessore                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Khulna road,Satkhira                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hospital Gate Shymnagar                                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kaligonj, jhenaidah                                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jail Road Jesore                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nolta Satlhira                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dhuliar Bazar Satkhira                                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C &amp; B Road Lohagara                                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uzirpur Bazar Assashuni Satkhira                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hospital Gate Narail                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kumri Bazar Lohagara Narail                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sheikhati Bazar, Narail                                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chalteghata Bazar Shyamnagar                                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kakbosia Bazar Assasuni                                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Khalashi Bazar Chowgacha                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chowrongi More, Khulna Road, Satkhira                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rupdia Bazar Jessore                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bagharpara Jessore                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JS22                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JS91                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JS73                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JS51                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JS84                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JS92                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JS14                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JS44                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JS53                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JS33                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JS52                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JS31                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JS54                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JS12                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JS21                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JS24                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV440-328103     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV440-463006     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV440-467048     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV440-445659     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV440-469487     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV440-469850     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV440-451099     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV440-473944     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV440-459896     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV440-476164     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV440-461819     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV440-462491     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV440-462021     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV440-462036     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV440-461796     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV440-463044     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV440-463702     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV440-457183     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV440-465161     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV440-465528     </t>
+  </si>
+  <si>
+    <t>04 Nov 2019</t>
+  </si>
+  <si>
+    <t>13 Sep 2020</t>
+  </si>
+  <si>
+    <t>21 Sep 2020</t>
+  </si>
+  <si>
+    <t>10 Aug 2020</t>
+  </si>
+  <si>
+    <t>26 Sep 2020</t>
+  </si>
+  <si>
+    <t>27 Sep 2020</t>
+  </si>
+  <si>
+    <t>20 Aug 2020</t>
+  </si>
+  <si>
+    <t>05 Oct 2020</t>
+  </si>
+  <si>
+    <t>07 Sep 2020</t>
+  </si>
+  <si>
+    <t>10 Oct 2020</t>
+  </si>
+  <si>
+    <t>11 Sep 2020</t>
+  </si>
+  <si>
+    <t>12 Sep 2020</t>
+  </si>
+  <si>
+    <t>14 Sep 2020</t>
+  </si>
+  <si>
+    <t>02 Sep 2020</t>
   </si>
   <si>
     <t>18 Sep 2020</t>
-  </si>
-  <si>
-    <t>06 Aug 2020</t>
-  </si>
-  <si>
-    <t>16 Jun 2020</t>
-  </si>
-  <si>
-    <t>27 Apr 2020</t>
-  </si>
-  <si>
-    <t>10 Aug 2020</t>
-  </si>
-  <si>
-    <t>31 Aug 2020</t>
-  </si>
-  <si>
-    <t>01 Sep 2020</t>
-  </si>
-  <si>
-    <t>02 Oct 2020</t>
-  </si>
-  <si>
-    <t>04 Oct 2020</t>
-  </si>
-  <si>
-    <t>08 Sep 2020</t>
-  </si>
-  <si>
-    <t>12 Aug 2020</t>
   </si>
 </sst>
 </file>
@@ -738,28 +774,28 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="E2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="F2" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="G2" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="H2">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>579</v>
+        <v>354</v>
       </c>
       <c r="J2">
-        <v>20124.56</v>
+        <v>37965.05</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -770,28 +806,28 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="E3" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="F3" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="G3" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="H3">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="I3">
-        <v>232</v>
+        <v>40</v>
       </c>
       <c r="J3">
-        <v>30531</v>
+        <v>4309.3</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -802,28 +838,28 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="E4" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="F4" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="G4" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="H4">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>62</v>
+        <v>32</v>
       </c>
       <c r="J4">
-        <v>1548.97</v>
+        <v>12174.16</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -834,28 +870,28 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="E5" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="F5" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="G5" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
       <c r="H5">
-        <v>150</v>
+        <v>45</v>
       </c>
       <c r="I5">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="J5">
-        <v>7068</v>
+        <v>19193.25</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -863,31 +899,31 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="E6" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="F6" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
       <c r="G6" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="H6">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="I6">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="J6">
-        <v>3991.58</v>
+        <v>12015.95</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -895,31 +931,31 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="E7" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="F7" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="G7" t="s">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="H7">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="I7">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="J7">
-        <v>11127.07</v>
+        <v>6099.06</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -927,31 +963,31 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E8" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="F8" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="G8" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="H8">
-        <v>150</v>
+        <v>45</v>
       </c>
       <c r="I8">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="J8">
-        <v>1854.52</v>
+        <v>286.66</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -959,31 +995,31 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="E9" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="F9" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="G9" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="I9">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="J9">
-        <v>10010</v>
+        <v>51924.81</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -991,31 +1027,31 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="E10" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="F10" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="G10" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
       <c r="H10">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="I10">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="J10">
-        <v>854</v>
+        <v>9758.530000000001</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1023,31 +1059,31 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="E11" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="F11" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="G11" t="s">
-        <v>99</v>
+        <v>114</v>
       </c>
       <c r="H11">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I11">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="J11">
-        <v>83834.25999999999</v>
+        <v>12055.35</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -1055,31 +1091,31 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" t="s">
+        <v>79</v>
+      </c>
+      <c r="F12" t="s">
+        <v>95</v>
+      </c>
+      <c r="G12" t="s">
+        <v>115</v>
+      </c>
+      <c r="H12">
+        <v>30</v>
+      </c>
+      <c r="I12">
         <v>12</v>
       </c>
-      <c r="C12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" t="s">
-        <v>58</v>
-      </c>
-      <c r="F12" t="s">
-        <v>80</v>
-      </c>
-      <c r="G12" t="s">
-        <v>100</v>
-      </c>
-      <c r="H12">
-        <v>150</v>
-      </c>
-      <c r="I12">
-        <v>25</v>
-      </c>
       <c r="J12">
-        <v>3431</v>
+        <v>5965.19</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -1087,31 +1123,31 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D13" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="E13" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="F13" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="G13" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="H13">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="I13">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="J13">
-        <v>90.97</v>
+        <v>10028.39</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1119,31 +1155,31 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="D14" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="E14" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="F14" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="G14" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="H14">
         <v>30</v>
       </c>
       <c r="I14">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="J14">
-        <v>17000</v>
+        <v>6049.62</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1151,31 +1187,31 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="D15" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="E15" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="F15" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="G15" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="H15">
         <v>30</v>
       </c>
       <c r="I15">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="J15">
-        <v>17540.62</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1183,31 +1219,31 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="D16" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="E16" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="F16" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="G16" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="H16">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="I16">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="J16">
-        <v>9461.07</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1215,31 +1251,31 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="D17" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="E17" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="F17" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="G17" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="I17">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="J17">
-        <v>369.62</v>
+        <v>6679.29</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1247,31 +1283,31 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="D18" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="E18" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="F18" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="G18" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="H18">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="I18">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="J18">
-        <v>2136.05</v>
+        <v>5380.45</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1279,31 +1315,31 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C19" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="D19" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="E19" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="F19" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="G19" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="H19">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="I19">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="J19">
-        <v>7500</v>
+        <v>56028.8</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1311,31 +1347,31 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C20" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="D20" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="E20" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="F20" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="G20" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="H20">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I20">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="J20">
-        <v>10804.62</v>
+        <v>13285.2</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1343,31 +1379,31 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="D21" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="E21" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="F21" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="G21" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="H21">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I21">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="J21">
-        <v>17657.25</v>
+        <v>5181.96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add new ndm informations in the chart
</commit_message>
<xml_diff>
--- a/Data/AgingMaturedTable.xlsx
+++ b/Data/AgingMaturedTable.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="109">
   <si>
     <t>Cust ID</t>
   </si>
@@ -43,316 +43,304 @@
     <t>Credit Amount</t>
   </si>
   <si>
-    <t>51052438752</t>
-  </si>
-  <si>
-    <t>51011137181</t>
-  </si>
-  <si>
-    <t>51011136733</t>
-  </si>
-  <si>
-    <t>51052138925</t>
-  </si>
-  <si>
-    <t>90000036187</t>
-  </si>
-  <si>
-    <t>90000023767</t>
-  </si>
-  <si>
-    <t>90000030972</t>
-  </si>
-  <si>
-    <t>51052149047</t>
-  </si>
-  <si>
-    <t>90000001093</t>
-  </si>
-  <si>
-    <t>51011136773</t>
-  </si>
-  <si>
-    <t>51051003724</t>
-  </si>
-  <si>
-    <t>90000007825</t>
-  </si>
-  <si>
-    <t>51011137476</t>
-  </si>
-  <si>
-    <t>51011117909</t>
-  </si>
-  <si>
-    <t>51051101305</t>
-  </si>
-  <si>
-    <t>51052100306</t>
-  </si>
-  <si>
-    <t>51051001866</t>
-  </si>
-  <si>
-    <t>51052103910</t>
-  </si>
-  <si>
-    <t>51011112125</t>
-  </si>
-  <si>
-    <t>Mega Medical Hall</t>
-  </si>
-  <si>
-    <t>AL Kayed Medcall hall</t>
-  </si>
-  <si>
-    <t>Khan Pharmacy</t>
-  </si>
-  <si>
-    <t>Munshi Drug House</t>
-  </si>
-  <si>
-    <t>Popular Medicine Corner 2</t>
-  </si>
-  <si>
-    <t>Shishu Medical Hall</t>
-  </si>
-  <si>
-    <t>Modina Medical Hall</t>
-  </si>
-  <si>
-    <t>Modern Diagnostic Center</t>
-  </si>
-  <si>
-    <t>Biplob Pharmacy</t>
-  </si>
-  <si>
-    <t>Moli Diagonostic Centre And Ho</t>
-  </si>
-  <si>
-    <t>Anil Medical Hall</t>
-  </si>
-  <si>
-    <t>Office Sales</t>
-  </si>
-  <si>
-    <t>Ummahani Hospital</t>
-  </si>
-  <si>
-    <t>Sohan Pharmacy</t>
-  </si>
-  <si>
-    <t>Dr Abdul Mutaleb Medical Hall</t>
-  </si>
-  <si>
-    <t>Alamgir Medical Hall</t>
-  </si>
-  <si>
-    <t>Bismillah Medical Hall</t>
-  </si>
-  <si>
-    <t>Satata Privet Clinic</t>
-  </si>
-  <si>
-    <t>Jogot Bandhu Pharmacy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Battala Bangla Bazar Bhola                                  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shordar Bari More Kalkine                                   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Janata Clab Badamtala Madaripur                             </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Munshi Drug House Battola Bazer Barisal                     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bangla Bazar,Barisal                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amanda Bazar,Sreepur,Barisal.                               </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Talukderhut, Eluhar hut, Swrupkati                          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hospital Gate Kalkini                                       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Talukder Bari Stand Donarkandi                              </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Takerhat Takerhat                                           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">llisha BatTola Bhola                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TDCL BARISAL                                                </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Upzala Road Rajoir                                          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Near Janata Pharmacy Hospitalm Gate Rajoir                  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shantirhat Bazar                                            </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bankerhat Bus Stand Bhola                                   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ilisha Bhola                                                </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Miarhat Bazar Swarupkathi Pirojpur                          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Takerhut North Side of Baily Bridge                         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">PB34                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MG54                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MG31                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BJ32                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BJ22                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BJ14                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BJ82                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MG52                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MG55                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MG32                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">PB31                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">INST                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MG33                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">PB32                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MG34                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV510-586791     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV510-587144     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV510-587610     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV510-588893     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV510-570555     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV510-589770     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV510-591062     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV510-590943     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV510-592349     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV510-592383     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV510-591818     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV510-592688     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV510-593069     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV510-592949     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV510-593229     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV510-594026     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV510-594107     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV510-594030     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV510-594764     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV510-596223     </t>
-  </si>
-  <si>
-    <t>31 Oct 2020</t>
-  </si>
-  <si>
-    <t>02 Nov 2020</t>
-  </si>
-  <si>
-    <t>04 Nov 2020</t>
-  </si>
-  <si>
-    <t>01 Oct 2020</t>
-  </si>
-  <si>
-    <t>06 Nov 2020</t>
-  </si>
-  <si>
-    <t>07 Nov 2020</t>
-  </si>
-  <si>
-    <t>09 Nov 2020</t>
-  </si>
-  <si>
-    <t>10 Nov 2020</t>
-  </si>
-  <si>
-    <t>11 Nov 2020</t>
-  </si>
-  <si>
-    <t>12 Nov 2020</t>
-  </si>
-  <si>
-    <t>14 Nov 2020</t>
-  </si>
-  <si>
-    <t>16 Nov 2020</t>
+    <t>43061104782</t>
+  </si>
+  <si>
+    <t>43061109178</t>
+  </si>
+  <si>
+    <t>4301901209</t>
+  </si>
+  <si>
+    <t>43061100638</t>
+  </si>
+  <si>
+    <t>90000042935</t>
+  </si>
+  <si>
+    <t>90000029247</t>
+  </si>
+  <si>
+    <t>43061101800</t>
+  </si>
+  <si>
+    <t>4201118395</t>
+  </si>
+  <si>
+    <t>43061109928</t>
+  </si>
+  <si>
+    <t>90000011704</t>
+  </si>
+  <si>
+    <t>43061109625</t>
+  </si>
+  <si>
+    <t>90000022393</t>
+  </si>
+  <si>
+    <t>4201117970</t>
+  </si>
+  <si>
+    <t>43061100760</t>
+  </si>
+  <si>
+    <t>90000030491</t>
+  </si>
+  <si>
+    <t>90000045498</t>
+  </si>
+  <si>
+    <t>43061109604</t>
+  </si>
+  <si>
+    <t>43061100261</t>
+  </si>
+  <si>
+    <t>90000041601</t>
+  </si>
+  <si>
+    <t>90000003726</t>
+  </si>
+  <si>
+    <t>Niramoy Pharmacy</t>
+  </si>
+  <si>
+    <t>Jesmin Parmacy</t>
+  </si>
+  <si>
+    <t>Ruma Pharmacy</t>
+  </si>
+  <si>
+    <t>Janasheba Pharmacy</t>
+  </si>
+  <si>
+    <t>Islamia Pharmacy</t>
+  </si>
+  <si>
+    <t>Amena Medical Stor</t>
+  </si>
+  <si>
+    <t>Renasase Med Centre</t>
+  </si>
+  <si>
+    <t>Molla Pharmacy</t>
+  </si>
+  <si>
+    <t>Sarder Medical</t>
+  </si>
+  <si>
+    <t>Chitholia Medical Store</t>
+  </si>
+  <si>
+    <t>Siddik Pharmacy</t>
+  </si>
+  <si>
+    <t>Rashida Medical Hall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bishwa Nath Medical </t>
+  </si>
+  <si>
+    <t>Kamal Pharmacy</t>
+  </si>
+  <si>
+    <t>Papri Pharmacy</t>
+  </si>
+  <si>
+    <t>Abdullah Pharmacy</t>
+  </si>
+  <si>
+    <t>Dr Eanur</t>
+  </si>
+  <si>
+    <t>Anower Medical Hall</t>
+  </si>
+  <si>
+    <t>Ritu Pharmacy</t>
+  </si>
+  <si>
+    <t>M S Selina Drug House</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chand Market Gorahmara Shimultala                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jhawdia Bazar Bittipara                                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Polish Line Magura                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amerchara more Parbotipur Horinakundo                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maspara Bazar,Pangsha.Rajbari                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allardarga Bazar.Doulatpur Kushtia.                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Khalishakundi Mirpur                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pangsha Bzaer Rajbari                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baliasisa Sherpur Mirpur                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chitholia Bazar, Mirpur                                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shauta Bridge Badh Bazar Panti Kushtia                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Polash Market Rajbari Road Boharpur Bazar Rajbari           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tatulia Bazar Baliakandi                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Goal Para Bazar Jhenaidha                                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roghunatpur.Chuadanga.                                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Halt Station Dorsona                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sahapur Andulbaria Jibonnagar                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Andol Baria Jibonnagar Chuadanga                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abdalpur Bazar,Kushtia.                                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fultola Chowrhas More                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">KC35                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">KC15                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FR71                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">KC44                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">KC82                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">KC34                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">KC33                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">KC25                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">KC83                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">KC45                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">KC53                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">KC13                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">KC11                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-502523     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-553218     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-557365     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-570783     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-571314     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-571506     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-571362     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-571195     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-571499     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-571429     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-559445     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-571596     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-571605     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-571961     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-571902     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-571975     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-571760     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-572066     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-571709     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV430-571669     </t>
+  </si>
+  <si>
+    <t>05 Aug 2020</t>
+  </si>
+  <si>
+    <t>19 Nov 2020</t>
+  </si>
+  <si>
+    <t>29 Nov 2020</t>
+  </si>
+  <si>
+    <t>02 Jan 2021</t>
+  </si>
+  <si>
+    <t>03 Jan 2021</t>
+  </si>
+  <si>
+    <t>04 Dec 2020</t>
+  </si>
+  <si>
+    <t>04 Jan 2021</t>
   </si>
 </sst>
 </file>
@@ -753,28 +741,28 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H2">
         <v>30</v>
       </c>
       <c r="I2">
-        <v>36</v>
+        <v>131</v>
       </c>
       <c r="J2">
-        <v>6666.73</v>
+        <v>5087.96</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -785,28 +773,28 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="H3">
         <v>30</v>
       </c>
       <c r="I3">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="J3">
-        <v>3200.34</v>
+        <v>3380.29</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -817,28 +805,28 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E4" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G4" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="H4">
         <v>30</v>
       </c>
       <c r="I4">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="J4">
-        <v>2138.06</v>
+        <v>6761.08</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -849,28 +837,28 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E5" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G5" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H5">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="J5">
-        <v>4032.09</v>
+        <v>11874.07</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -881,28 +869,28 @@
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E6" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F6" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G6" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="H6">
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="I6">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="J6">
-        <v>24140.23</v>
+        <v>50025.66</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -913,28 +901,28 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E7" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H7">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I7">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="J7">
-        <v>3009.26</v>
+        <v>30047.96</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -945,28 +933,28 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E8" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G8" t="s">
         <v>106</v>
       </c>
       <c r="H8">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I8">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="J8">
-        <v>14768.83</v>
+        <v>19879.04</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -977,28 +965,28 @@
         <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E9" t="s">
         <v>73</v>
       </c>
       <c r="F9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G9" t="s">
         <v>106</v>
       </c>
       <c r="H9">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I9">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="J9">
-        <v>14207.86</v>
+        <v>14879.15</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1009,28 +997,28 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D10" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E10" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F10" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H10">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I10">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="J10">
-        <v>9994.91</v>
+        <v>12027.12</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1041,28 +1029,28 @@
         <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E11" t="s">
         <v>75</v>
       </c>
       <c r="F11" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H11">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I11">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="J11">
-        <v>4720</v>
+        <v>6994.36</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -1073,16 +1061,16 @@
         <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E12" t="s">
         <v>76</v>
       </c>
       <c r="F12" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G12" t="s">
         <v>107</v>
@@ -1091,10 +1079,10 @@
         <v>30</v>
       </c>
       <c r="I12">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="J12">
-        <v>2895.77</v>
+        <v>5036.26</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -1105,28 +1093,28 @@
         <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D13" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E13" t="s">
         <v>77</v>
       </c>
       <c r="F13" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G13" t="s">
         <v>108</v>
       </c>
       <c r="H13">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I13">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="J13">
-        <v>2112.24</v>
+        <v>20061.52</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1137,28 +1125,28 @@
         <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H14">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I14">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="J14">
-        <v>4453.57</v>
+        <v>20022.54</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1166,31 +1154,31 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D15" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E15" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F15" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H15">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I15">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="J15">
-        <v>2112.24</v>
+        <v>14906.48</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1198,31 +1186,31 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D16" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E16" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F16" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H16">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I16">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="J16">
-        <v>2000.48</v>
+        <v>14283.94</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1230,31 +1218,31 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D17" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E17" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="F17" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G17" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H17">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I17">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="J17">
-        <v>14931</v>
+        <v>10026.5</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1262,31 +1250,31 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D18" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E18" t="s">
         <v>79</v>
       </c>
       <c r="F18" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G18" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H18">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I18">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="J18">
-        <v>9906.049999999999</v>
+        <v>9697.969999999999</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1294,31 +1282,31 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C19" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D19" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E19" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="F19" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G19" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H19">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I19">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="J19">
-        <v>204.28</v>
+        <v>9628.540000000001</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1326,31 +1314,31 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C20" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D20" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E20" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="F20" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G20" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="H20">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I20">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="J20">
-        <v>2015.87</v>
+        <v>6672.56</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1358,31 +1346,31 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C21" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D21" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E21" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F21" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G21" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="H21">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I21">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="J21">
-        <v>2441.79</v>
+        <v>3531.01</v>
       </c>
     </row>
   </sheetData>

</xml_diff>